<commit_message>
Add Steam World templates
</commit_message>
<xml_diff>
--- a/RR_templates.xlsx
+++ b/RR_templates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="18375" windowHeight="8625"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="18375" windowHeight="8625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Surface" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
     <author>Jadon Wade</author>
   </authors>
   <commentList>
-    <comment ref="O2" authorId="0" shapeId="0">
+    <comment ref="R2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0">
+    <comment ref="S2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="143">
   <si>
     <t>Zeonium</t>
   </si>
@@ -563,6 +563,15 @@
   </si>
   <si>
     <t>Spodumene</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Steam (CO2)</t>
+  </si>
+  <si>
+    <t>Steam (N2)</t>
   </si>
 </sst>
 </file>
@@ -799,7 +808,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -887,10 +896,11 @@
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -1174,11 +1184,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E13" sqref="E13"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1188,9 +1198,10 @@
     <col min="6" max="6" width="10.125" customWidth="1"/>
     <col min="7" max="7" width="10.875" customWidth="1"/>
     <col min="8" max="9" width="12.25" customWidth="1"/>
+    <col min="17" max="19" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1243,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1286,7 +1297,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1326,8 +1337,11 @@
       <c r="N4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1344,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1364,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1431,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1472,7 +1486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1507,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1565,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1606,7 +1620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1620,7 +1634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1658,7 +1672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1708,25 +1722,25 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="39">
         <v>18</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="39">
         <v>18</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="39">
         <v>11</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="39">
         <v>13</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="39">
         <v>11</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="39">
         <v>9</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="39">
         <v>5</v>
       </c>
       <c r="I18">
@@ -1746,25 +1760,25 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="39">
         <v>13</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="39">
         <v>24</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="39">
         <v>6</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="39">
         <v>5</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="39">
         <v>5</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="39">
         <v>7</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="39">
         <v>5</v>
       </c>
       <c r="I19">
@@ -2414,7 +2428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F11" sqref="F11"/>
+      <selection pane="topRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2753,13 +2767,13 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="39">
         <v>22</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="39">
         <v>25</v>
       </c>
-      <c r="K16" s="40">
+      <c r="K16" s="39">
         <v>12</v>
       </c>
     </row>
@@ -2767,11 +2781,11 @@
       <c r="A17" t="s">
         <v>139</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="39">
         <v>22</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40">
+      <c r="J17" s="39"/>
+      <c r="K17" s="39">
         <v>8</v>
       </c>
     </row>
@@ -2779,11 +2793,11 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="40">
-        <v>3</v>
-      </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
+      <c r="I18" s="39">
+        <v>3</v>
+      </c>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2804,11 +2818,11 @@
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40">
+      <c r="I19" s="39"/>
+      <c r="J19" s="39">
         <v>52</v>
       </c>
-      <c r="K19" s="40">
+      <c r="K19" s="39">
         <v>60</v>
       </c>
     </row>
@@ -3068,37 +3082,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="12.25" customWidth="1"/>
-    <col min="9" max="10" width="12.375" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="14.25" customWidth="1"/>
-    <col min="13" max="13" width="12.625" customWidth="1"/>
-    <col min="14" max="16" width="12.125" customWidth="1"/>
-    <col min="17" max="17" width="12.875" customWidth="1"/>
-    <col min="18" max="18" width="12.125" customWidth="1"/>
-    <col min="19" max="19" width="10.75" customWidth="1"/>
-    <col min="20" max="20" width="11.5" customWidth="1"/>
-    <col min="21" max="21" width="10.25" customWidth="1"/>
-    <col min="23" max="23" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="12.625" customWidth="1"/>
-    <col min="27" max="27" width="12.375" customWidth="1"/>
-    <col min="28" max="28" width="12.875" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="12.25" customWidth="1"/>
+    <col min="12" max="13" width="12.375" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="14.25" customWidth="1"/>
+    <col min="16" max="16" width="12.625" customWidth="1"/>
+    <col min="17" max="19" width="12.125" customWidth="1"/>
+    <col min="20" max="20" width="12.875" customWidth="1"/>
+    <col min="21" max="21" width="12.125" customWidth="1"/>
+    <col min="22" max="22" width="10.75" customWidth="1"/>
+    <col min="23" max="23" width="11.5" customWidth="1"/>
+    <col min="24" max="24" width="10.25" customWidth="1"/>
+    <col min="26" max="26" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="12.625" customWidth="1"/>
+    <col min="30" max="30" width="12.375" customWidth="1"/>
+    <col min="31" max="31" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -3109,79 +3124,88 @@
         <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="R1" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="40"/>
+      <c r="T1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:Q2" si="0">SUM(B4:B18)</f>
+        <f t="shared" ref="B2:T2" si="0">SUM(B4:B18)</f>
         <v>93</v>
       </c>
       <c r="C2" s="1">
@@ -3189,220 +3213,235 @@
         <v>92</v>
       </c>
       <c r="D2" s="33">
+        <f t="shared" ref="D2:E2" si="1">SUM(D4:D18)</f>
+        <v>85.118380062305292</v>
+      </c>
+      <c r="E2" s="33">
+        <f t="shared" si="1"/>
+        <v>89.059190031152639</v>
+      </c>
+      <c r="F2" s="33">
+        <f t="shared" si="0"/>
+        <v>90.223364485981307</v>
+      </c>
+      <c r="G2" s="33">
         <f t="shared" si="0"/>
         <v>95.007788161993773</v>
       </c>
-      <c r="E2" s="1">
+      <c r="H2" s="1">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="F2" s="1">
+      <c r="I2" s="1">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="G2" s="4">
+      <c r="J2" s="4">
         <f t="shared" si="0"/>
         <v>92.003115264797515</v>
       </c>
-      <c r="H2" s="4">
+      <c r="K2" s="4">
         <f t="shared" si="0"/>
         <v>90.006230529595015</v>
       </c>
-      <c r="I2" s="4">
+      <c r="L2" s="4">
         <f t="shared" si="0"/>
         <v>92.003115264797515</v>
       </c>
-      <c r="J2" s="4">
+      <c r="M2" s="4">
         <f t="shared" si="0"/>
         <v>96.000778816199372</v>
       </c>
-      <c r="K2" s="4">
+      <c r="N2" s="4">
         <f t="shared" si="0"/>
         <v>96.615264797507791</v>
       </c>
-      <c r="L2" s="4">
+      <c r="O2" s="4">
         <f t="shared" si="0"/>
         <v>94.115264797507791</v>
       </c>
-      <c r="M2" s="4">
+      <c r="P2" s="4">
         <f t="shared" si="0"/>
         <v>99.121495327102807</v>
       </c>
-      <c r="N2" s="4">
+      <c r="Q2" s="4">
         <f t="shared" si="0"/>
         <v>99.121495327102807</v>
       </c>
-      <c r="O2" s="34">
+      <c r="R2" s="34">
         <f t="shared" si="0"/>
         <v>91.862149532710276</v>
       </c>
-      <c r="P2" s="34">
+      <c r="S2" s="34">
         <f t="shared" si="0"/>
         <v>96.109034267912776</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="T2" s="4">
         <f t="shared" si="0"/>
         <v>100.00778816199377</v>
       </c>
-      <c r="S2" s="4">
-        <f>SUM(S4:S18)</f>
+      <c r="V2" s="4">
+        <f>SUM(V4:V18)</f>
         <v>90.109034267912776</v>
       </c>
-      <c r="T2" s="4">
-        <f>SUM(T4:T18)</f>
+      <c r="W2" s="4">
+        <f>SUM(W4:W18)</f>
         <v>95.116822429906534</v>
       </c>
-      <c r="U2" s="4">
-        <f>SUM(U4:U18)</f>
+      <c r="X2" s="4">
+        <f>SUM(X4:X18)</f>
         <v>99.13239875389408</v>
       </c>
-      <c r="W2" s="4">
-        <f t="shared" ref="W2:AB2" si="1">SUM(W4:W18)</f>
+      <c r="Z2" s="4">
+        <f t="shared" ref="Z2:AE2" si="2">SUM(Z4:Z18)</f>
         <v>95.109034267912776</v>
       </c>
-      <c r="X2" s="4">
-        <f t="shared" si="1"/>
+      <c r="AA2" s="4">
+        <f t="shared" si="2"/>
         <v>98.031152647975077</v>
       </c>
-      <c r="Y2" s="4">
-        <f t="shared" si="1"/>
+      <c r="AB2" s="4">
+        <f t="shared" si="2"/>
         <v>92.031152647975077</v>
       </c>
-      <c r="Z2" s="4">
-        <f t="shared" si="1"/>
+      <c r="AC2" s="4">
+        <f t="shared" si="2"/>
         <v>11.004672897196262</v>
       </c>
-      <c r="AA2" s="4">
-        <f t="shared" si="1"/>
+      <c r="AD2" s="4">
+        <f t="shared" si="2"/>
         <v>94.60280373831776</v>
       </c>
-      <c r="AB2" s="4">
-        <f t="shared" si="1"/>
+      <c r="AE2" s="4">
+        <f t="shared" si="2"/>
         <v>98.085669781931472</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="37"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="37"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="O4" s="35">
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="35">
         <v>0.1</v>
       </c>
-      <c r="P4" s="37">
-        <v>4</v>
-      </c>
-      <c r="S4">
+      <c r="S4" s="37">
+        <v>4</v>
+      </c>
+      <c r="V4">
         <v>1</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="Z4">
         <v>5</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>1.5</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5" s="35">
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="35">
         <v>1</v>
       </c>
-      <c r="P5" s="37"/>
-      <c r="Q5">
+      <c r="S5" s="37"/>
+      <c r="T5">
         <v>1</v>
       </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5">
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
         <v>5</v>
       </c>
-      <c r="U5">
+      <c r="X5">
         <v>9</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>70</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>70</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>1</v>
       </c>
-      <c r="AA5">
-        <v>3</v>
-      </c>
-      <c r="AB5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD5">
+        <v>3</v>
+      </c>
+      <c r="AE5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
-      <c r="O6" s="35"/>
-      <c r="P6" s="37"/>
-      <c r="S6">
+      <c r="R6" s="35"/>
+      <c r="S6" s="37"/>
+      <c r="V6">
         <v>1</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>1</v>
       </c>
-      <c r="AA6">
-        <v>2</v>
-      </c>
-      <c r="AB6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD6">
+        <v>2</v>
+      </c>
+      <c r="AE6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="P7" s="37"/>
-      <c r="AB7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R7" s="35"/>
+      <c r="S7" s="37"/>
+      <c r="AE7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3412,343 +3451,367 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>20</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
         <v>91</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
         <v>1</v>
       </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8" s="35">
-        <v>2</v>
-      </c>
-      <c r="P8" s="37">
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8" s="35">
+        <v>2</v>
+      </c>
+      <c r="S8" s="37">
         <v>5</v>
       </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="S8">
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="V8">
         <v>1</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>1</v>
       </c>
-      <c r="W8">
-        <v>2</v>
-      </c>
-      <c r="AA8">
+      <c r="Z8">
+        <v>2</v>
+      </c>
+      <c r="AD8">
         <v>5</v>
       </c>
-      <c r="AB8">
+      <c r="AE8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" ref="D9" si="2">D12/642</f>
+        <f>(D12+D17)/642</f>
+        <v>0.11838006230529595</v>
+      </c>
+      <c r="E9" s="3">
+        <f>(E12+E17)/642</f>
+        <v>5.9190031152647975E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <f>(F12+F17)/642</f>
+        <v>2.336448598130841E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9" si="3">G12/642</f>
         <v>7.7881619937694704E-3</v>
       </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9:U9" si="3">G12/642</f>
+      <c r="J9" s="3">
+        <f t="shared" ref="J9:X9" si="4">J12/642</f>
         <v>3.1152647975077881E-3</v>
       </c>
-      <c r="H9" s="3">
-        <f t="shared" si="3"/>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
         <v>6.2305295950155761E-3</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="3"/>
+      <c r="L9" s="3">
+        <f t="shared" si="4"/>
         <v>3.1152647975077881E-3</v>
       </c>
-      <c r="J9" s="3">
-        <f>J12/642</f>
+      <c r="M9" s="3">
+        <f>M12/642</f>
         <v>7.7881619937694702E-4</v>
       </c>
-      <c r="K9" s="3">
-        <f t="shared" si="3"/>
+      <c r="N9" s="3">
+        <f t="shared" si="4"/>
         <v>0.11526479750778816</v>
       </c>
-      <c r="L9" s="3">
-        <f t="shared" si="3"/>
+      <c r="O9" s="3">
+        <f t="shared" si="4"/>
         <v>0.11526479750778816</v>
       </c>
-      <c r="M9" s="3">
-        <f t="shared" si="3"/>
+      <c r="P9" s="3">
+        <f t="shared" si="4"/>
         <v>0.12149532710280374</v>
       </c>
-      <c r="N9" s="3">
-        <f t="shared" si="3"/>
+      <c r="Q9" s="3">
+        <f t="shared" si="4"/>
         <v>0.12149532710280374</v>
       </c>
-      <c r="O9" s="36">
-        <f t="shared" si="3"/>
+      <c r="R9" s="36">
+        <f t="shared" si="4"/>
         <v>0.11214953271028037</v>
       </c>
-      <c r="P9" s="38">
-        <f t="shared" si="3"/>
+      <c r="S9" s="38">
+        <f t="shared" si="4"/>
         <v>0.10903426791277258</v>
       </c>
-      <c r="Q9" s="3">
-        <f>Q12/642</f>
+      <c r="T9" s="3">
+        <f>T12/642</f>
         <v>7.7881619937694704E-3</v>
       </c>
-      <c r="S9" s="3">
-        <f t="shared" si="3"/>
+      <c r="V9" s="3">
+        <f t="shared" si="4"/>
         <v>0.10903426791277258</v>
       </c>
-      <c r="T9" s="3">
-        <f t="shared" si="3"/>
+      <c r="W9" s="3">
+        <f t="shared" si="4"/>
         <v>0.11682242990654206</v>
       </c>
-      <c r="U9" s="3">
-        <f t="shared" si="3"/>
+      <c r="X9" s="3">
+        <f t="shared" si="4"/>
         <v>0.13239875389408098</v>
       </c>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3">
-        <f>W12/642</f>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3">
+        <f>Z12/642</f>
         <v>0.10903426791277258</v>
       </c>
-      <c r="X9" s="3">
-        <f t="shared" ref="X9:Z9" si="4">X12/642</f>
+      <c r="AA9" s="3">
+        <f t="shared" ref="AA9:AC9" si="5">AA12/642</f>
         <v>3.1152647975077882E-2</v>
       </c>
-      <c r="Y9" s="3">
-        <f t="shared" si="4"/>
+      <c r="AB9" s="3">
+        <f t="shared" si="5"/>
         <v>3.1152647975077882E-2</v>
       </c>
-      <c r="Z9" s="3">
-        <f t="shared" si="4"/>
+      <c r="AC9" s="3">
+        <f t="shared" si="5"/>
         <v>4.6728971962616819E-3</v>
       </c>
-      <c r="AA9" s="3">
-        <f>AA12/642</f>
+      <c r="AD9" s="3">
+        <f>AD12/642</f>
         <v>0.10280373831775701</v>
       </c>
-      <c r="AB9" s="3">
-        <f>AB12/642</f>
+      <c r="AE9" s="3">
+        <f>AE12/642</f>
         <v>8.566978193146417E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="38"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="38"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-      <c r="Y10">
-        <v>2</v>
-      </c>
-      <c r="Z10">
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="J11">
+      <c r="F11">
+        <v>0.2</v>
+      </c>
+      <c r="M11">
         <v>0.5</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>12</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>10</v>
       </c>
-      <c r="M11">
+      <c r="P11">
         <v>10</v>
       </c>
-      <c r="N11">
+      <c r="Q11">
         <v>10</v>
       </c>
-      <c r="O11" s="35">
+      <c r="R11" s="35">
         <v>10</v>
       </c>
-      <c r="P11" s="37">
+      <c r="S11" s="37">
         <v>9</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <v>90</v>
       </c>
-      <c r="S11">
+      <c r="V11">
         <v>7</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>7</v>
       </c>
-      <c r="U11">
+      <c r="X11">
         <v>5</v>
       </c>
-      <c r="W11">
+      <c r="Z11">
         <v>10</v>
-      </c>
-      <c r="X11">
-        <v>8</v>
-      </c>
-      <c r="Z11">
-        <v>2</v>
       </c>
       <c r="AA11">
         <v>8</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>8</v>
+      </c>
+      <c r="AE11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>5</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
       <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
         <v>0.5</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>74</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <v>74</v>
       </c>
-      <c r="M12">
+      <c r="P12">
         <v>78</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <v>78</v>
       </c>
-      <c r="O12" s="35">
+      <c r="R12" s="35">
         <v>72</v>
       </c>
-      <c r="P12" s="37">
+      <c r="S12" s="37">
         <v>70</v>
       </c>
-      <c r="Q12">
+      <c r="T12">
         <v>5</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>70</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>75</v>
       </c>
-      <c r="U12">
+      <c r="X12">
         <v>85</v>
       </c>
-      <c r="W12">
+      <c r="Z12">
         <v>70</v>
       </c>
-      <c r="X12">
+      <c r="AA12">
         <v>20</v>
       </c>
-      <c r="Y12">
+      <c r="AB12">
         <v>20</v>
       </c>
-      <c r="Z12">
-        <v>3</v>
-      </c>
-      <c r="AA12">
+      <c r="AC12">
+        <v>3</v>
+      </c>
+      <c r="AD12">
         <v>66</v>
       </c>
-      <c r="AB12">
+      <c r="AE12">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="J13">
         <v>6</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
-      <c r="M13">
-        <v>4</v>
-      </c>
       <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13" s="35">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13" s="35">
         <v>0.05</v>
       </c>
-      <c r="P13" s="37">
-        <v>4</v>
-      </c>
-      <c r="S13">
+      <c r="S13" s="37">
+        <v>4</v>
+      </c>
+      <c r="V13">
         <v>1</v>
       </c>
-      <c r="W13">
+      <c r="Z13">
         <v>5</v>
       </c>
-      <c r="AA13">
+      <c r="AD13">
         <v>3.5</v>
       </c>
-      <c r="AB13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AE13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3758,44 +3821,47 @@
       <c r="C14">
         <v>74</v>
       </c>
-      <c r="D14">
+      <c r="F14">
+        <v>66</v>
+      </c>
+      <c r="G14">
         <v>50</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <v>80</v>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>75</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>85</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>90</v>
       </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
       <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="P14">
         <v>1</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <v>1</v>
       </c>
-      <c r="O14" s="35">
+      <c r="R14" s="35">
         <v>5</v>
       </c>
-      <c r="P14" s="37">
-        <v>3</v>
-      </c>
-      <c r="S14">
-        <v>2</v>
-      </c>
-      <c r="T14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S14" s="37">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>2</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3805,46 +3871,55 @@
       <c r="D15">
         <v>9</v>
       </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
       <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="M15">
         <v>90</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
       </c>
       <c r="N15">
         <v>1</v>
       </c>
-      <c r="O15" s="35">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="35">
         <v>0.6</v>
       </c>
-      <c r="P15" s="37"/>
-      <c r="S15">
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <v>2</v>
-      </c>
-      <c r="AA15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S15" s="37"/>
+      <c r="V15">
+        <v>2</v>
+      </c>
+      <c r="W15">
+        <v>2</v>
+      </c>
+      <c r="AD15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <v>1</v>
       </c>
-      <c r="O16" s="35"/>
-      <c r="P16" s="37"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R16" s="35"/>
+      <c r="S16" s="37"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -3855,236 +3930,260 @@
         <v>1</v>
       </c>
       <c r="D17">
+        <v>76</v>
+      </c>
+      <c r="E17">
+        <v>38</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
         <v>5</v>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
       <c r="M17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
-      <c r="O17" s="35">
-        <v>1</v>
-      </c>
-      <c r="P17" s="37">
-        <v>1</v>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>4</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
-      <c r="W17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R17" s="35">
+        <v>1</v>
+      </c>
+      <c r="S17" s="37">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="O18" s="35"/>
-      <c r="P18" s="37"/>
-      <c r="S18">
-        <v>2</v>
-      </c>
-      <c r="T18">
+      <c r="R18" s="35"/>
+      <c r="S18" s="37"/>
+      <c r="V18">
+        <v>2</v>
+      </c>
+      <c r="W18">
         <v>1</v>
       </c>
-      <c r="AA18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ref="B21:O21" si="5">SUM(B23:B31)</f>
+        <f t="shared" ref="B21:R21" si="6">SUM(B23:B31)</f>
         <v>10</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="6"/>
+        <v>31.5</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="E21" s="1">
-        <f t="shared" si="5"/>
+      <c r="H21" s="1">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="F21" s="1">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" si="5"/>
+      <c r="I21" s="1">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="H21" s="1">
-        <f t="shared" si="5"/>
+      <c r="K21" s="1">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="I21" s="1">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="J21" s="1">
-        <f>SUM(J23:J31)</f>
+      <c r="L21" s="1">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="M21" s="1">
+        <f>SUM(M23:M31)</f>
         <v>97</v>
       </c>
-      <c r="K21" s="1">
-        <f t="shared" si="5"/>
+      <c r="N21" s="1">
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
-      <c r="L21" s="1">
-        <f t="shared" si="5"/>
+      <c r="O21" s="1">
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
-      <c r="M21" s="1">
-        <f t="shared" si="5"/>
+      <c r="P21" s="1">
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
-      <c r="N21" s="1">
-        <f t="shared" si="5"/>
+      <c r="Q21" s="1">
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
-      <c r="O21" s="1">
-        <f t="shared" si="5"/>
+      <c r="R21" s="1">
+        <f t="shared" si="6"/>
         <v>97.05</v>
       </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1">
-        <f>SUM(Q23:Q31)</f>
-        <v>93</v>
-      </c>
-      <c r="S21" s="1">
-        <f>SUM(S23:S31)</f>
-        <v>95</v>
-      </c>
+      <c r="S21" s="1"/>
       <c r="T21" s="1">
         <f>SUM(T23:T31)</f>
+        <v>93</v>
+      </c>
+      <c r="V21" s="1">
+        <f>SUM(V23:V31)</f>
         <v>95</v>
       </c>
-      <c r="U21" s="1">
-        <f>SUM(U23:U31)</f>
+      <c r="W21" s="1">
+        <f>SUM(W23:W31)</f>
+        <v>95</v>
+      </c>
+      <c r="X21" s="1">
+        <f>SUM(X23:X31)</f>
         <v>99</v>
       </c>
-      <c r="W21" s="1">
-        <f t="shared" ref="W21:AB21" si="6">SUM(W23:W31)</f>
+      <c r="Z21" s="1">
+        <f t="shared" ref="Z21:AE21" si="7">SUM(Z23:Z31)</f>
         <v>92</v>
       </c>
-      <c r="X21" s="1">
-        <f t="shared" si="6"/>
+      <c r="AA21" s="1">
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="Y21" s="1">
-        <f t="shared" si="6"/>
+      <c r="AB21" s="1">
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="Z21" s="1">
-        <f t="shared" si="6"/>
+      <c r="AC21" s="1">
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="AA21" s="1">
-        <f t="shared" si="6"/>
+      <c r="AD21" s="1">
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
-      <c r="AB21" s="1">
-        <f t="shared" si="6"/>
+      <c r="AE21" s="1">
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23">
-        <v>2</v>
-      </c>
+      <c r="N23" s="35"/>
       <c r="O23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="S23">
+      <c r="P23" s="35"/>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="V23">
         <v>1</v>
       </c>
-      <c r="T23">
+      <c r="W23">
         <v>5</v>
       </c>
-      <c r="U23">
+      <c r="X23">
         <v>9</v>
       </c>
-      <c r="X23">
+      <c r="AA23">
         <v>70</v>
       </c>
-      <c r="Y23">
+      <c r="AB23">
         <v>70</v>
       </c>
-      <c r="Z23">
+      <c r="AC23">
         <v>1</v>
       </c>
-      <c r="AA23">
-        <v>3</v>
-      </c>
-      <c r="AB23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD23">
+        <v>3</v>
+      </c>
+      <c r="AE23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="J24">
+      <c r="F24">
         <v>0.5</v>
       </c>
-      <c r="K24">
+      <c r="M24">
+        <v>0.5</v>
+      </c>
+      <c r="N24">
         <v>12</v>
       </c>
-      <c r="L24">
+      <c r="O24">
         <v>10</v>
       </c>
-      <c r="O24" s="35">
+      <c r="R24" s="35">
         <v>9</v>
       </c>
-      <c r="Q24">
+      <c r="T24">
         <v>90</v>
       </c>
-      <c r="S24">
+      <c r="V24">
         <v>7</v>
       </c>
-      <c r="T24">
+      <c r="W24">
         <v>7</v>
       </c>
-      <c r="U24">
+      <c r="X24">
         <v>5</v>
       </c>
-      <c r="W24">
+      <c r="Z24">
         <v>10</v>
       </c>
-      <c r="Z24">
-        <v>2</v>
-      </c>
-      <c r="AA24">
+      <c r="AC24">
+        <v>2</v>
+      </c>
+      <c r="AD24">
         <v>8</v>
       </c>
-      <c r="AB24">
+      <c r="AE24">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -4094,50 +4193,53 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="J25">
         <v>6</v>
       </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
       <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="N25">
         <v>1</v>
       </c>
-      <c r="L25">
+      <c r="O25">
         <v>6</v>
       </c>
-      <c r="M25">
-        <v>4</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
-      <c r="O25" s="35">
-        <v>4</v>
-      </c>
-      <c r="S25">
-        <v>4</v>
-      </c>
-      <c r="T25">
-        <v>2</v>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>3</v>
+      </c>
+      <c r="R25" s="35">
+        <v>4</v>
+      </c>
+      <c r="V25">
+        <v>4</v>
       </c>
       <c r="W25">
+        <v>2</v>
+      </c>
+      <c r="Z25">
         <v>6</v>
       </c>
-      <c r="AA25">
+      <c r="AD25">
         <v>5</v>
       </c>
-      <c r="AB25">
+      <c r="AE25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4147,168 +4249,171 @@
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
         <v>6</v>
       </c>
-      <c r="F26">
-        <v>3</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
       <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
         <v>1</v>
       </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
       <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="P26">
         <v>1</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26" s="35">
-        <v>0.05</v>
       </c>
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="S26">
-        <v>2</v>
+      <c r="R26" s="35">
+        <v>0.05</v>
       </c>
       <c r="T26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="J27">
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="M27">
         <v>90</v>
       </c>
-      <c r="M27">
+      <c r="P27">
         <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27" s="35">
-        <v>2</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
-      <c r="S27">
+      <c r="R27" s="35">
         <v>2</v>
       </c>
       <c r="T27">
         <v>1</v>
       </c>
-      <c r="AA27">
-        <v>3</v>
-      </c>
-      <c r="AB27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="V27">
+        <v>2</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>3</v>
+      </c>
+      <c r="AE27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="G28">
         <v>6</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <v>4</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
       <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
         <v>0.5</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>74</v>
       </c>
-      <c r="L28">
+      <c r="O28">
         <v>70</v>
       </c>
-      <c r="M28">
+      <c r="P28">
         <v>78</v>
       </c>
-      <c r="N28">
+      <c r="Q28">
         <v>78</v>
       </c>
-      <c r="O28" s="35">
+      <c r="R28" s="35">
         <v>78</v>
       </c>
-      <c r="Q28">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="S28">
+      <c r="V28">
         <v>70</v>
       </c>
-      <c r="T28">
+      <c r="W28">
         <v>75</v>
       </c>
-      <c r="U28">
+      <c r="X28">
         <v>85</v>
       </c>
-      <c r="W28">
+      <c r="Z28">
         <v>70</v>
       </c>
-      <c r="Y28">
+      <c r="AB28">
         <v>20</v>
       </c>
-      <c r="Z28">
+      <c r="AC28">
         <v>10</v>
       </c>
-      <c r="AA28">
+      <c r="AD28">
         <v>75</v>
       </c>
-      <c r="AB28">
+      <c r="AE28">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-      <c r="O29" s="35"/>
-      <c r="S29">
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="R29" s="35"/>
+      <c r="V29">
         <v>5</v>
       </c>
-      <c r="T29">
-        <v>2</v>
-      </c>
-      <c r="X29">
+      <c r="W29">
+        <v>2</v>
+      </c>
+      <c r="AA29">
         <v>20</v>
       </c>
-      <c r="AB29">
+      <c r="AE29">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -4319,34 +4424,43 @@
         <v>1</v>
       </c>
       <c r="D30">
+        <v>76</v>
+      </c>
+      <c r="E30">
+        <v>38</v>
+      </c>
+      <c r="F30">
+        <v>15</v>
+      </c>
+      <c r="G30">
         <v>5</v>
       </c>
-      <c r="G30">
+      <c r="J30">
         <v>1</v>
       </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>2</v>
-      </c>
       <c r="M30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
-      <c r="O30" s="35">
+      <c r="O30">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+      <c r="Q30">
         <v>1</v>
       </c>
-      <c r="W30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R30" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -4360,51 +4474,60 @@
         <v>2</v>
       </c>
       <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
         <v>6</v>
       </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="I31">
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="L31">
         <v>1</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>4</v>
       </c>
       <c r="M31">
         <v>1</v>
       </c>
       <c r="N31">
-        <v>3</v>
-      </c>
-      <c r="O31" s="35">
-        <v>3</v>
-      </c>
-      <c r="S31">
-        <v>4</v>
-      </c>
-      <c r="T31">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31" s="35">
+        <v>3</v>
+      </c>
+      <c r="V31">
+        <v>4</v>
       </c>
       <c r="W31">
-        <v>4</v>
-      </c>
-      <c r="AA31">
-        <v>4</v>
-      </c>
-      <c r="AB31">
+        <v>2</v>
+      </c>
+      <c r="Z31">
+        <v>4</v>
+      </c>
+      <c r="AD31">
+        <v>4</v>
+      </c>
+      <c r="AE31">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Add templates and tab for deep crust resources concept
</commit_message>
<xml_diff>
--- a/RR_templates.xlsx
+++ b/RR_templates.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22320" yWindow="0" windowWidth="18375" windowHeight="8625" activeTab="1"/>
+    <workbookView xWindow="23250" yWindow="0" windowWidth="18375" windowHeight="8625" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Surface" sheetId="1" r:id="rId1"/>
-    <sheet name="Ocean" sheetId="2" r:id="rId2"/>
-    <sheet name="Atmo" sheetId="3" r:id="rId3"/>
-    <sheet name="Exo Bands" sheetId="4" r:id="rId4"/>
+    <sheet name="Crust" sheetId="1" r:id="rId1"/>
+    <sheet name="Deep Crust" sheetId="5" r:id="rId2"/>
+    <sheet name="Ocean" sheetId="2" r:id="rId3"/>
+    <sheet name="Atmo" sheetId="3" r:id="rId4"/>
+    <sheet name="Exo Bands" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -249,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
   <si>
     <t>Zeonium</t>
   </si>
@@ -708,6 +709,54 @@
   </si>
   <si>
     <t>Iron</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>Tritium</t>
+  </si>
+  <si>
+    <t>Thorium</t>
+  </si>
+  <si>
+    <t>Sulfur</t>
+  </si>
+  <si>
+    <t>Iron Oxide</t>
+  </si>
+  <si>
+    <t>Carbonatite</t>
+  </si>
+  <si>
+    <t>Alkaline</t>
+  </si>
+  <si>
+    <t>Mafic/Basaltic</t>
+  </si>
+  <si>
+    <t>Felsic</t>
+  </si>
+  <si>
+    <t>Deep Rock</t>
+  </si>
+  <si>
+    <t>Deep Magma</t>
+  </si>
+  <si>
+    <t>Dirt</t>
+  </si>
+  <si>
+    <t>Carbon Dioxide</t>
+  </si>
+  <si>
+    <t>Carbon Monoxide</t>
+  </si>
+  <si>
+    <t>Helium-3</t>
+  </si>
+  <si>
+    <t>Lithium</t>
   </si>
 </sst>
 </file>
@@ -720,9 +769,16 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -869,8 +925,22 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,6 +987,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -951,111 +1027,128 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Comma 2" xfId="3"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1337,7 +1430,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2680,10 +2773,399 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.625" style="42" customWidth="1"/>
+    <col min="2" max="10" width="11.25" style="42" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+    </row>
+    <row r="2" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+      <c r="B2" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="43">
+        <f>SUM(B5:B25)</f>
+        <v>99.7</v>
+      </c>
+      <c r="C3" s="43">
+        <f t="shared" ref="C3:J3" si="0">SUM(C5:C25)</f>
+        <v>86.8</v>
+      </c>
+      <c r="D3" s="43">
+        <f t="shared" si="0"/>
+        <v>73.8</v>
+      </c>
+      <c r="E3" s="43">
+        <f t="shared" si="0"/>
+        <v>92.8</v>
+      </c>
+      <c r="F3" s="43">
+        <f t="shared" si="0"/>
+        <v>95.7</v>
+      </c>
+      <c r="G3" s="43">
+        <f t="shared" si="0"/>
+        <v>99.8</v>
+      </c>
+      <c r="H3" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="42">
+        <v>15</v>
+      </c>
+      <c r="C5" s="42">
+        <v>4</v>
+      </c>
+      <c r="D5" s="42">
+        <v>5</v>
+      </c>
+      <c r="E5" s="42">
+        <v>3</v>
+      </c>
+      <c r="F5" s="42">
+        <v>5.5</v>
+      </c>
+      <c r="G5" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="42">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="42">
+        <v>1</v>
+      </c>
+      <c r="C9" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="D9" s="42">
+        <v>4</v>
+      </c>
+      <c r="E9" s="42">
+        <v>1</v>
+      </c>
+      <c r="F9" s="42">
+        <v>1</v>
+      </c>
+      <c r="G9" s="42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="42">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="42">
+        <v>8.1</v>
+      </c>
+      <c r="C13" s="42">
+        <v>16</v>
+      </c>
+      <c r="D13" s="42">
+        <v>3</v>
+      </c>
+      <c r="E13" s="42">
+        <v>2</v>
+      </c>
+      <c r="F13" s="42">
+        <v>42</v>
+      </c>
+      <c r="G13" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="42">
+        <v>8</v>
+      </c>
+      <c r="D14" s="42">
+        <v>3</v>
+      </c>
+      <c r="E14" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="42">
+        <v>1.9</v>
+      </c>
+      <c r="G14" s="42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="42">
+        <v>7.1</v>
+      </c>
+      <c r="C15" s="42">
+        <v>8</v>
+      </c>
+      <c r="D15" s="42">
+        <v>13</v>
+      </c>
+      <c r="E15" s="42">
+        <v>5</v>
+      </c>
+      <c r="F15" s="42">
+        <v>8</v>
+      </c>
+      <c r="G15" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="49">
+        <v>67</v>
+      </c>
+      <c r="C16" s="49">
+        <v>48</v>
+      </c>
+      <c r="D16" s="49">
+        <v>42</v>
+      </c>
+      <c r="E16" s="49">
+        <v>31</v>
+      </c>
+      <c r="F16" s="49">
+        <v>36</v>
+      </c>
+      <c r="G16" s="49">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="42">
+        <v>1</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1</v>
+      </c>
+      <c r="D17" s="42">
+        <v>1</v>
+      </c>
+      <c r="E17" s="42">
+        <v>1</v>
+      </c>
+      <c r="F17" s="42">
+        <v>1</v>
+      </c>
+      <c r="G17" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="50">
+        <f>SUM(100-B3)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="C26" s="50">
+        <f t="shared" ref="C26:J26" si="1">SUM(100-C3)</f>
+        <v>13.200000000000003</v>
+      </c>
+      <c r="D26" s="50">
+        <f t="shared" si="1"/>
+        <v>26.200000000000003</v>
+      </c>
+      <c r="E26" s="50">
+        <f t="shared" si="1"/>
+        <v>7.2000000000000028</v>
+      </c>
+      <c r="F26" s="50">
+        <f t="shared" si="1"/>
+        <v>4.2999999999999972</v>
+      </c>
+      <c r="G26" s="50">
+        <f t="shared" si="1"/>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="H26" s="50">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I26" s="50">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J26" s="50">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L26" sqref="L26"/>
     </sheetView>
@@ -3434,7 +3916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH39"/>
   <sheetViews>
@@ -5130,7 +5612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q75"/>
   <sheetViews>

</xml_diff>